<commit_message>
Réalisation code importer excel et générer .mat des variables (quelques points à corriger encore)
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Template_Caract_Vehicle.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Template_Caract_Vehicle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC87CC6-B9EF-4B9A-925D-43E8695AA07F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639C23CF-9140-4E9C-8F95-B4686CD06AA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="15400" xr2:uid="{3D022185-A71E-4154-B100-A37570255104}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15400" xr2:uid="{3D022185-A71E-4154-B100-A37570255104}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Paramètre</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Concept_2</t>
-  </si>
-  <si>
-    <t>Concept_3</t>
   </si>
   <si>
     <t>m_p (kg)</t>
@@ -597,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B42D80E-A6FA-4D33-9CF0-11D96E9603BE}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +605,7 @@
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -626,361 +623,466 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>1.236</v>
+      </c>
+      <c r="D3">
+        <v>1.236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>1.236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.165</v>
+      </c>
+      <c r="D4">
+        <v>1.165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>1.165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.575</v>
+      </c>
+      <c r="D5">
+        <v>1.575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>1.575</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.78749999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>0.78749999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.52</v>
+      </c>
+      <c r="D7">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.77110000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>0.77110000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="D11">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>5.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.03</v>
+      </c>
+      <c r="D13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.313</v>
+      </c>
+      <c r="D14">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C15">
-        <v>0.313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>39</v>
       </c>
       <c r="C16">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="D16">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>40</v>
       </c>
       <c r="C17">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.42</v>
+      </c>
+      <c r="D17">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>41</v>
       </c>
       <c r="C18">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+        <v>0.31</v>
+      </c>
+      <c r="D18">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>2.13</v>
+      </c>
+      <c r="D20">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C22">
-        <v>2.13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D22">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+      <c r="D23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.9</v>
+      </c>
+      <c r="D26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>9000</v>
+      </c>
+      <c r="D27">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
       <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>13500</v>
+      </c>
+      <c r="D28">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>13500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.3125</v>
+      </c>
+      <c r="D34">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C35">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>0.47370000000000001</v>
+      </c>
+      <c r="D36">
+        <v>0.47370000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37">
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C39">
-        <v>0.47370000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
+        <f>(C17*C15+C18*C16+C23*C24)/C40</f>
+        <v>0.34016666666666673</v>
+      </c>
+      <c r="D39">
+        <f>(D17*D15+D18*D16+D23*D24)/D40</f>
+        <v>0.34016666666666673</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <f>C15+C16+C24</f>
+        <v>300</v>
+      </c>
+      <c r="D40">
+        <f>D15+D16+D24</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43">
-        <f>(C18*C16+C19*C17+C25*C26)/C44</f>
-        <v>0.34016666666666673</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44">
-        <f>C16+C17+C26</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
         <v>24</v>
       </c>
-      <c r="C45">
+      <c r="C41">
+        <v>0.1</v>
+      </c>
+      <c r="D41">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A29:A41"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rangement, changement mineur de l'arborescence et ajout de documents
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Template_Caract_Vehicle.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Template_Caract_Vehicle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B5835E-4FD5-40FA-95D7-54211F42FACD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF89726-33CF-4C52-8A90-70D5DDBE8E24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15400" xr2:uid="{3D022185-A71E-4154-B100-A37570255104}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Paramètre</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Engine_Type</t>
+  </si>
+  <si>
+    <t>Concept_3</t>
   </si>
 </sst>
 </file>
@@ -594,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B42D80E-A6FA-4D33-9CF0-11D96E9603BE}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +608,7 @@
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>30</v>
       </c>
@@ -623,8 +626,11 @@
       <c r="D2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -637,8 +643,11 @@
       <c r="D3">
         <v>1.236</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>1.236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>35</v>
@@ -649,8 +658,11 @@
       <c r="D4">
         <v>1.165</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>1.165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>36</v>
@@ -661,8 +673,11 @@
       <c r="D5">
         <v>1.575</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>1.575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>37</v>
@@ -673,8 +688,11 @@
       <c r="D6">
         <v>0.78749999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>0.78749999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>38</v>
@@ -685,8 +703,11 @@
       <c r="D7">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>29</v>
@@ -697,8 +718,11 @@
       <c r="D8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>16</v>
@@ -709,8 +733,11 @@
       <c r="D9">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -721,8 +748,11 @@
       <c r="D10">
         <v>0.77110000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>0.77110000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>6</v>
@@ -733,8 +763,11 @@
       <c r="D11">
         <v>5.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>7</v>
@@ -745,8 +778,11 @@
       <c r="D12">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>8</v>
@@ -757,8 +793,11 @@
       <c r="D13">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>9</v>
@@ -769,8 +808,11 @@
       <c r="D14">
         <v>0.313</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>39</v>
@@ -781,8 +823,11 @@
       <c r="D15">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>40</v>
@@ -793,8 +838,11 @@
       <c r="D16">
         <v>215</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>41</v>
@@ -805,8 +853,11 @@
       <c r="D17">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>42</v>
@@ -817,8 +868,11 @@
       <c r="D18">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -829,10 +883,13 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>3</v>
@@ -843,8 +900,11 @@
       <c r="D20">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>4</v>
@@ -855,8 +915,11 @@
       <c r="D21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>43</v>
@@ -867,8 +930,11 @@
       <c r="D22">
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>44</v>
@@ -879,8 +945,11 @@
       <c r="D23">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
         <v>45</v>
@@ -891,8 +960,11 @@
       <c r="D24">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>28</v>
       </c>
@@ -905,8 +977,11 @@
       <c r="D25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" t="s">
         <v>17</v>
@@ -917,8 +992,11 @@
       <c r="D26">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" t="s">
         <v>18</v>
@@ -929,8 +1007,11 @@
       <c r="D27">
         <v>9000</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>19</v>
@@ -941,8 +1022,11 @@
       <c r="D28">
         <v>13500</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>20</v>
@@ -953,8 +1037,11 @@
       <c r="D29">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" t="s">
         <v>21</v>
@@ -965,8 +1052,11 @@
       <c r="D30">
         <v>1111</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>10</v>
@@ -977,8 +1067,11 @@
       <c r="D31">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" t="s">
         <v>11</v>
@@ -989,8 +1082,11 @@
       <c r="D32">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>12</v>
@@ -1001,8 +1097,11 @@
       <c r="D33">
         <v>1111</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>13</v>
@@ -1013,8 +1112,11 @@
       <c r="D34">
         <v>0.3125</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" t="s">
         <v>14</v>
@@ -1025,8 +1127,11 @@
       <c r="D35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>15</v>
@@ -1037,8 +1142,11 @@
       <c r="D36">
         <v>0.47370000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <v>0.47370000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" t="s">
         <v>22</v>
@@ -1049,8 +1157,11 @@
       <c r="D37">
         <v>1111</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" t="s">
         <v>23</v>
@@ -1061,8 +1172,11 @@
       <c r="D38">
         <v>1111</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>27</v>
       </c>
@@ -1077,8 +1191,12 @@
         <f>(D17*D15+D18*D16+D23*D24)/D40</f>
         <v>0.34016666666666673</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39">
+        <f>(E17*E15+E18*E16+E23*E24)/E40</f>
+        <v>0.34016666666666673</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>47</v>
       </c>
@@ -1090,8 +1208,12 @@
         <f>D15+D16+D24</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40">
+        <f>E15+E16+E24</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>24</v>
       </c>
@@ -1099,6 +1221,9 @@
         <v>0.1</v>
       </c>
       <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>